<commit_message>
test(excel): Improve test cases coverall.
</commit_message>
<xml_diff>
--- a/test/test_files/excel.xlsx
+++ b/test/test_files/excel.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FEA363-6DB1-9647-A18D-EDF3E631C4A7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4D1D1E-8581-6044-9A56-8605391A5718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>inputs</t>
   </si>
@@ -35,12 +41,15 @@
   <si>
     <t>Intermediate</t>
   </si>
+  <si>
+    <t>defaults</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,15 +395,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +413,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -414,11 +426,14 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <f>B2/B3</f>
-        <v>4</v>
+        <f>B2/B3+D2</f>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>6</v>
       </c>
@@ -427,11 +442,15 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>C2*A2</f>
-        <v>8</v>
+        <f>C2*A2+D3</f>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f>1+D2</f>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>5</v>
       </c>
@@ -440,8 +459,12 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <f>B3^C2</f>
-        <v>16</v>
+        <f>B3^C2+D4</f>
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <f>1+D3</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(excel), #82: Add inverse of simple references.
</commit_message>
<xml_diff>
--- a/test/test_files/excel.xlsx
+++ b/test/test_files/excel.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4D1D1E-8581-6044-9A56-8605391A5718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD971235-43FF-8B40-B2F5-7047CD57547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="INPUT_A">DATA!$A$2</definedName>
+    <definedName name="INPUT_B">DATA!$A$3</definedName>
+    <definedName name="INPUT_C">DATA!$A$4</definedName>
+  </definedNames>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,12 +403,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -433,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -450,7 +455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>

</xml_diff>